<commit_message>
maj diagramme d'exigence et classe et diapo
</commit_message>
<xml_diff>
--- a/documentation/oral/FinalGanttAllJEAN.xlsx
+++ b/documentation/oral/FinalGanttAllJEAN.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F25D84-0AB9-4FC2-8E7D-BE4AF5D91E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003C1A78-823D-457E-B9F7-B3CDAB85D856}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -825,6 +825,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="22" fillId="0" borderId="2" xfId="21" applyFont="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -866,9 +869,6 @@
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="22" fillId="0" borderId="2" xfId="21" applyFont="1" applyProtection="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -1294,10 +1294,10 @@
   <dimension ref="A1:HC31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="G5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="BM24" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="AL8" sqref="AL8"/>
+      <selection pane="bottomRight" activeCell="DE24" sqref="DE24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.21875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1327,35 +1327,35 @@
       <c r="L1" s="33">
         <v>1</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
       <c r="P1" s="34">
         <v>2</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="R1" s="41"/>
-      <c r="S1" s="41"/>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
       <c r="T1" s="35">
         <v>3</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
       <c r="X1" s="36">
         <v>4</v>
       </c>
-      <c r="Y1" s="41" t="s">
+      <c r="Y1" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
+      <c r="Z1" s="42"/>
+      <c r="AA1" s="42"/>
     </row>
     <row r="2" spans="1:211" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F2" s="17"/>
@@ -1370,66 +1370,66 @@
         <v>1</v>
       </c>
       <c r="N2" s="11"/>
-      <c r="O2" s="49" t="s">
+      <c r="O2" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="52"/>
       <c r="T2" s="12"/>
-      <c r="U2" s="49" t="s">
+      <c r="U2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="51"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="52"/>
       <c r="Y2" s="13"/>
-      <c r="Z2" s="42" t="s">
+      <c r="Z2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="53"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="54"/>
       <c r="AD2" s="14"/>
-      <c r="AE2" s="42" t="s">
+      <c r="AE2" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="43"/>
-      <c r="AI2" s="43"/>
-      <c r="AJ2" s="43"/>
-      <c r="AK2" s="53"/>
+      <c r="AF2" s="44"/>
+      <c r="AG2" s="44"/>
+      <c r="AH2" s="44"/>
+      <c r="AI2" s="44"/>
+      <c r="AJ2" s="44"/>
+      <c r="AK2" s="54"/>
       <c r="AL2" s="15"/>
-      <c r="AM2" s="42" t="s">
+      <c r="AM2" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="AN2" s="43"/>
-      <c r="AO2" s="43"/>
-      <c r="AP2" s="43"/>
-      <c r="AQ2" s="43"/>
-      <c r="AR2" s="43"/>
-      <c r="AS2" s="43"/>
-      <c r="AT2" s="43"/>
+      <c r="AN2" s="44"/>
+      <c r="AO2" s="44"/>
+      <c r="AP2" s="44"/>
+      <c r="AQ2" s="44"/>
+      <c r="AR2" s="44"/>
+      <c r="AS2" s="44"/>
+      <c r="AT2" s="44"/>
     </row>
     <row r="3" spans="1:211" s="7" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="46" t="s">
+      <c r="G3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="46" t="s">
+      <c r="H3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="46" t="s">
+      <c r="I3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="48" t="s">
+      <c r="K3" s="49" t="s">
         <v>6</v>
       </c>
       <c r="L3" s="16" t="s">
@@ -1456,808 +1456,808 @@
       <c r="AE3" s="6"/>
     </row>
     <row r="4" spans="1:211" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="45"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="55">
+      <c r="F4" s="46"/>
+      <c r="G4" s="48"/>
+      <c r="H4" s="48"/>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="41">
         <v>1</v>
       </c>
-      <c r="M4" s="55">
+      <c r="M4" s="41">
         <f>L4+1</f>
         <v>2</v>
       </c>
-      <c r="N4" s="55">
+      <c r="N4" s="41">
         <f t="shared" ref="N4:BY4" si="0">M4+1</f>
         <v>3</v>
       </c>
-      <c r="O4" s="55">
+      <c r="O4" s="41">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="P4" s="55">
+      <c r="P4" s="41">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="Q4" s="55">
+      <c r="Q4" s="41">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="R4" s="55">
+      <c r="R4" s="41">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="S4" s="55">
+      <c r="S4" s="41">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="T4" s="55">
+      <c r="T4" s="41">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="U4" s="55">
+      <c r="U4" s="41">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="V4" s="55">
+      <c r="V4" s="41">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="W4" s="55">
+      <c r="W4" s="41">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="X4" s="55">
+      <c r="X4" s="41">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="Y4" s="55">
+      <c r="Y4" s="41">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="Z4" s="55">
+      <c r="Z4" s="41">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="AA4" s="55">
+      <c r="AA4" s="41">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="AB4" s="55">
+      <c r="AB4" s="41">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="AC4" s="55">
+      <c r="AC4" s="41">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="AD4" s="55">
+      <c r="AD4" s="41">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="AE4" s="55">
+      <c r="AE4" s="41">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="AF4" s="55">
+      <c r="AF4" s="41">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="AG4" s="55">
+      <c r="AG4" s="41">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="AH4" s="55">
+      <c r="AH4" s="41">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="AI4" s="55">
+      <c r="AI4" s="41">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="AJ4" s="55">
+      <c r="AJ4" s="41">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="AK4" s="55">
+      <c r="AK4" s="41">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="AL4" s="55">
+      <c r="AL4" s="41">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="AM4" s="55">
+      <c r="AM4" s="41">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="AN4" s="55">
+      <c r="AN4" s="41">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="AO4" s="55">
+      <c r="AO4" s="41">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="AP4" s="55">
+      <c r="AP4" s="41">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="AQ4" s="55">
+      <c r="AQ4" s="41">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="AR4" s="55">
+      <c r="AR4" s="41">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="AS4" s="55">
+      <c r="AS4" s="41">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="AT4" s="55">
+      <c r="AT4" s="41">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="AU4" s="55">
+      <c r="AU4" s="41">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="AV4" s="55">
+      <c r="AV4" s="41">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="AW4" s="55">
+      <c r="AW4" s="41">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="AX4" s="55">
+      <c r="AX4" s="41">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="AY4" s="55">
+      <c r="AY4" s="41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="AZ4" s="55">
+      <c r="AZ4" s="41">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="BA4" s="55">
+      <c r="BA4" s="41">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="BB4" s="55">
+      <c r="BB4" s="41">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="BC4" s="55">
+      <c r="BC4" s="41">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="BD4" s="55">
+      <c r="BD4" s="41">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="BE4" s="55">
+      <c r="BE4" s="41">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="BF4" s="55">
+      <c r="BF4" s="41">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="BG4" s="55">
+      <c r="BG4" s="41">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="BH4" s="55">
+      <c r="BH4" s="41">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="BI4" s="55">
+      <c r="BI4" s="41">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="BJ4" s="55">
+      <c r="BJ4" s="41">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="BK4" s="55">
+      <c r="BK4" s="41">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="BL4" s="55">
+      <c r="BL4" s="41">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="BM4" s="55">
+      <c r="BM4" s="41">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="BN4" s="55">
+      <c r="BN4" s="41">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="BO4" s="55">
+      <c r="BO4" s="41">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="BP4" s="55">
+      <c r="BP4" s="41">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="BQ4" s="55">
+      <c r="BQ4" s="41">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="BR4" s="55">
+      <c r="BR4" s="41">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="BS4" s="55">
+      <c r="BS4" s="41">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="BT4" s="55">
+      <c r="BT4" s="41">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="BU4" s="55">
+      <c r="BU4" s="41">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="BV4" s="55">
+      <c r="BV4" s="41">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="BW4" s="55">
+      <c r="BW4" s="41">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="BX4" s="55">
+      <c r="BX4" s="41">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="BY4" s="55">
+      <c r="BY4" s="41">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="BZ4" s="55">
+      <c r="BZ4" s="41">
         <f t="shared" ref="BZ4:EK4" si="1">BY4+1</f>
         <v>67</v>
       </c>
-      <c r="CA4" s="55">
+      <c r="CA4" s="41">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="CB4" s="55">
+      <c r="CB4" s="41">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="CC4" s="55">
+      <c r="CC4" s="41">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="CD4" s="55">
+      <c r="CD4" s="41">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="CE4" s="55">
+      <c r="CE4" s="41">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="CF4" s="55">
+      <c r="CF4" s="41">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="CG4" s="55">
+      <c r="CG4" s="41">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="CH4" s="55">
+      <c r="CH4" s="41">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="CI4" s="55">
+      <c r="CI4" s="41">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="CJ4" s="55">
+      <c r="CJ4" s="41">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="CK4" s="55">
+      <c r="CK4" s="41">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="CL4" s="55">
+      <c r="CL4" s="41">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="CM4" s="55">
+      <c r="CM4" s="41">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="CN4" s="55">
+      <c r="CN4" s="41">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="CO4" s="55">
+      <c r="CO4" s="41">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="CP4" s="55">
+      <c r="CP4" s="41">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="CQ4" s="55">
+      <c r="CQ4" s="41">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="CR4" s="55">
+      <c r="CR4" s="41">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="CS4" s="55">
+      <c r="CS4" s="41">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="CT4" s="55">
+      <c r="CT4" s="41">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="CU4" s="55">
+      <c r="CU4" s="41">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="CV4" s="55">
+      <c r="CV4" s="41">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="CW4" s="55">
+      <c r="CW4" s="41">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="CX4" s="55">
+      <c r="CX4" s="41">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="CY4" s="55">
+      <c r="CY4" s="41">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="CZ4" s="55">
+      <c r="CZ4" s="41">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="DA4" s="55">
+      <c r="DA4" s="41">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="DB4" s="55">
+      <c r="DB4" s="41">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="DC4" s="55">
+      <c r="DC4" s="41">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="DD4" s="55">
+      <c r="DD4" s="41">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="DE4" s="55">
+      <c r="DE4" s="41">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="DF4" s="55">
+      <c r="DF4" s="41">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="DG4" s="55">
+      <c r="DG4" s="41">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="DH4" s="55">
+      <c r="DH4" s="41">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="DI4" s="55">
+      <c r="DI4" s="41">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="DJ4" s="55">
+      <c r="DJ4" s="41">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="DK4" s="55">
+      <c r="DK4" s="41">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="DL4" s="55">
+      <c r="DL4" s="41">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="DM4" s="55">
+      <c r="DM4" s="41">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="DN4" s="55">
+      <c r="DN4" s="41">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="DO4" s="55">
+      <c r="DO4" s="41">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="DP4" s="55">
+      <c r="DP4" s="41">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="DQ4" s="55">
+      <c r="DQ4" s="41">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="DR4" s="55">
+      <c r="DR4" s="41">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="DS4" s="55">
+      <c r="DS4" s="41">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="DT4" s="55">
+      <c r="DT4" s="41">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="DU4" s="55">
+      <c r="DU4" s="41">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="DV4" s="55">
+      <c r="DV4" s="41">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="DW4" s="55">
+      <c r="DW4" s="41">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="DX4" s="55">
+      <c r="DX4" s="41">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="DY4" s="55">
+      <c r="DY4" s="41">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="DZ4" s="55">
+      <c r="DZ4" s="41">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="EA4" s="55">
+      <c r="EA4" s="41">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="EB4" s="55">
+      <c r="EB4" s="41">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="EC4" s="55">
+      <c r="EC4" s="41">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="ED4" s="55">
+      <c r="ED4" s="41">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="EE4" s="55">
+      <c r="EE4" s="41">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="EF4" s="55">
+      <c r="EF4" s="41">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="EG4" s="55">
+      <c r="EG4" s="41">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="EH4" s="55">
+      <c r="EH4" s="41">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="EI4" s="55">
+      <c r="EI4" s="41">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="EJ4" s="55">
+      <c r="EJ4" s="41">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="EK4" s="55">
+      <c r="EK4" s="41">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="EL4" s="55">
+      <c r="EL4" s="41">
         <f t="shared" ref="EL4:GW4" si="2">EK4+1</f>
         <v>131</v>
       </c>
-      <c r="EM4" s="55">
+      <c r="EM4" s="41">
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
-      <c r="EN4" s="55">
+      <c r="EN4" s="41">
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-      <c r="EO4" s="55">
+      <c r="EO4" s="41">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="EP4" s="55">
+      <c r="EP4" s="41">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="EQ4" s="55">
+      <c r="EQ4" s="41">
         <f t="shared" si="2"/>
         <v>136</v>
       </c>
-      <c r="ER4" s="55">
+      <c r="ER4" s="41">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
-      <c r="ES4" s="55">
+      <c r="ES4" s="41">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="ET4" s="55">
+      <c r="ET4" s="41">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
-      <c r="EU4" s="55">
+      <c r="EU4" s="41">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="EV4" s="55">
+      <c r="EV4" s="41">
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
-      <c r="EW4" s="55">
+      <c r="EW4" s="41">
         <f t="shared" si="2"/>
         <v>142</v>
       </c>
-      <c r="EX4" s="55">
+      <c r="EX4" s="41">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-      <c r="EY4" s="55">
+      <c r="EY4" s="41">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="EZ4" s="55">
+      <c r="EZ4" s="41">
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
-      <c r="FA4" s="55">
+      <c r="FA4" s="41">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="FB4" s="55">
+      <c r="FB4" s="41">
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
-      <c r="FC4" s="55">
+      <c r="FC4" s="41">
         <f t="shared" si="2"/>
         <v>148</v>
       </c>
-      <c r="FD4" s="55">
+      <c r="FD4" s="41">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
-      <c r="FE4" s="55">
+      <c r="FE4" s="41">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="FF4" s="55">
+      <c r="FF4" s="41">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="FG4" s="55">
+      <c r="FG4" s="41">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-      <c r="FH4" s="55">
+      <c r="FH4" s="41">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
-      <c r="FI4" s="55">
+      <c r="FI4" s="41">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="FJ4" s="55">
+      <c r="FJ4" s="41">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-      <c r="FK4" s="55">
+      <c r="FK4" s="41">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
-      <c r="FL4" s="55">
+      <c r="FL4" s="41">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
-      <c r="FM4" s="55">
+      <c r="FM4" s="41">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="FN4" s="55">
+      <c r="FN4" s="41">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-      <c r="FO4" s="55">
+      <c r="FO4" s="41">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="FP4" s="55">
+      <c r="FP4" s="41">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
-      <c r="FQ4" s="55">
+      <c r="FQ4" s="41">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-      <c r="FR4" s="55">
+      <c r="FR4" s="41">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
-      <c r="FS4" s="55">
+      <c r="FS4" s="41">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="FT4" s="55">
+      <c r="FT4" s="41">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="FU4" s="55">
+      <c r="FU4" s="41">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
-      <c r="FV4" s="55">
+      <c r="FV4" s="41">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="FW4" s="55">
+      <c r="FW4" s="41">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
-      <c r="FX4" s="55">
+      <c r="FX4" s="41">
         <f t="shared" si="2"/>
         <v>169</v>
       </c>
-      <c r="FY4" s="55">
+      <c r="FY4" s="41">
         <f t="shared" si="2"/>
         <v>170</v>
       </c>
-      <c r="FZ4" s="55">
+      <c r="FZ4" s="41">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
-      <c r="GA4" s="55">
+      <c r="GA4" s="41">
         <f t="shared" si="2"/>
         <v>172</v>
       </c>
-      <c r="GB4" s="55">
+      <c r="GB4" s="41">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
-      <c r="GC4" s="55">
+      <c r="GC4" s="41">
         <f t="shared" si="2"/>
         <v>174</v>
       </c>
-      <c r="GD4" s="55">
+      <c r="GD4" s="41">
         <f t="shared" si="2"/>
         <v>175</v>
       </c>
-      <c r="GE4" s="55">
+      <c r="GE4" s="41">
         <f t="shared" si="2"/>
         <v>176</v>
       </c>
-      <c r="GF4" s="55">
+      <c r="GF4" s="41">
         <f t="shared" si="2"/>
         <v>177</v>
       </c>
-      <c r="GG4" s="55">
+      <c r="GG4" s="41">
         <f t="shared" si="2"/>
         <v>178</v>
       </c>
-      <c r="GH4" s="55">
+      <c r="GH4" s="41">
         <f t="shared" si="2"/>
         <v>179</v>
       </c>
-      <c r="GI4" s="55">
+      <c r="GI4" s="41">
         <f t="shared" si="2"/>
         <v>180</v>
       </c>
-      <c r="GJ4" s="55">
+      <c r="GJ4" s="41">
         <f t="shared" si="2"/>
         <v>181</v>
       </c>
-      <c r="GK4" s="55">
+      <c r="GK4" s="41">
         <f t="shared" si="2"/>
         <v>182</v>
       </c>
-      <c r="GL4" s="55">
+      <c r="GL4" s="41">
         <f t="shared" si="2"/>
         <v>183</v>
       </c>
-      <c r="GM4" s="55">
+      <c r="GM4" s="41">
         <f t="shared" si="2"/>
         <v>184</v>
       </c>
-      <c r="GN4" s="55">
+      <c r="GN4" s="41">
         <f t="shared" si="2"/>
         <v>185</v>
       </c>
-      <c r="GO4" s="55">
+      <c r="GO4" s="41">
         <f t="shared" si="2"/>
         <v>186</v>
       </c>
-      <c r="GP4" s="55">
+      <c r="GP4" s="41">
         <f t="shared" si="2"/>
         <v>187</v>
       </c>
-      <c r="GQ4" s="55">
+      <c r="GQ4" s="41">
         <f t="shared" si="2"/>
         <v>188</v>
       </c>
-      <c r="GR4" s="55">
+      <c r="GR4" s="41">
         <f t="shared" si="2"/>
         <v>189</v>
       </c>
-      <c r="GS4" s="55">
+      <c r="GS4" s="41">
         <f t="shared" si="2"/>
         <v>190</v>
       </c>
-      <c r="GT4" s="55">
+      <c r="GT4" s="41">
         <f t="shared" si="2"/>
         <v>191</v>
       </c>
-      <c r="GU4" s="55">
+      <c r="GU4" s="41">
         <f t="shared" si="2"/>
         <v>192</v>
       </c>
-      <c r="GV4" s="55">
+      <c r="GV4" s="41">
         <f t="shared" si="2"/>
         <v>193</v>
       </c>
-      <c r="GW4" s="55">
+      <c r="GW4" s="41">
         <f t="shared" si="2"/>
         <v>194</v>
       </c>
-      <c r="GX4" s="55">
+      <c r="GX4" s="41">
         <f t="shared" ref="GX4:HC4" si="3">GW4+1</f>
         <v>195</v>
       </c>
-      <c r="GY4" s="55">
+      <c r="GY4" s="41">
         <f t="shared" si="3"/>
         <v>196</v>
       </c>
-      <c r="GZ4" s="55">
+      <c r="GZ4" s="41">
         <f t="shared" si="3"/>
         <v>197</v>
       </c>
-      <c r="HA4" s="55">
+      <c r="HA4" s="41">
         <f t="shared" si="3"/>
         <v>198</v>
       </c>
-      <c r="HB4" s="55">
+      <c r="HB4" s="41">
         <f t="shared" si="3"/>
         <v>199</v>
       </c>
-      <c r="HC4" s="55">
+      <c r="HC4" s="41">
         <f t="shared" si="3"/>
         <v>200</v>
       </c>

</xml_diff>